<commit_message>
Starting importfromexcel.js script to manage uploading data to MongoDB from Excel
</commit_message>
<xml_diff>
--- a/backend/datamanagement/data/importfromexceltestdata.xlsx
+++ b/backend/datamanagement/data/importfromexceltestdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acris/Projects/akkaxedf/backend/datamanagement/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Documents/DTY/Projet 1 - AKKA Technologies/Akka x EDF repo/backend/datamanagement/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Chat</t>
   </si>
@@ -42,6 +42,21 @@
   </si>
   <si>
     <t>Lion</t>
+  </si>
+  <si>
+    <t>Colonne parfois vide</t>
+  </si>
+  <si>
+    <t>Rempli</t>
+  </si>
+  <si>
+    <t>Repas</t>
+  </si>
+  <si>
+    <t>Thon</t>
+  </si>
+  <si>
+    <t>Viande</t>
   </si>
 </sst>
 </file>
@@ -356,44 +371,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>14</v>
       </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>10</v>
       </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>